<commit_message>
code for clustering PCA/area
</commit_message>
<xml_diff>
--- a/_CIPW/CIPW/time_rocktype/1_rocktype_area_time.xlsx
+++ b/_CIPW/CIPW/time_rocktype/1_rocktype_area_time.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sebastian\Desktop\python_map\New\Vistelius_1995_OCR\_CIPW\CIPW\time_rocktype\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2705D3DE-7812-4C22-9E37-4319259B8B1A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C717E7C8-45E5-45FB-8B43-0104F6CA853C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{B7820438-7F70-491A-BCC9-34F83339C664}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="294" uniqueCount="30">
   <si>
     <t>time</t>
   </si>
@@ -111,6 +111,21 @@
   </si>
   <si>
     <t>Area5</t>
+  </si>
+  <si>
+    <t>totaal area1</t>
+  </si>
+  <si>
+    <t>totaal area2</t>
+  </si>
+  <si>
+    <t>totaal area3</t>
+  </si>
+  <si>
+    <t>totaal area4</t>
+  </si>
+  <si>
+    <t>totaal area5</t>
   </si>
 </sst>
 </file>
@@ -230,7 +245,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -271,6 +286,10 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standaard" xfId="0" builtinId="0"/>
@@ -585,10 +604,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C4F7BD3F-7764-4EBA-9637-34201CA977B0}">
-  <dimension ref="A1:S99"/>
+  <dimension ref="A1:S127"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E27" sqref="E27"/>
+    <sheetView tabSelected="1" topLeftCell="B100" workbookViewId="0">
+      <selection activeCell="L122" sqref="L122"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -599,7 +618,7 @@
     <col min="8" max="8" width="37.21875" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="5.5546875" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="6.44140625" customWidth="1"/>
-    <col min="12" max="12" width="37.21875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="42.33203125" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="5.5546875" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="5.6640625" customWidth="1"/>
     <col min="15" max="15" width="5.5546875" customWidth="1"/>
@@ -661,7 +680,7 @@
         <v>512</v>
       </c>
       <c r="F4">
-        <f>E4/$E$11*100</f>
+        <f t="shared" ref="F4:F11" si="0">E4/$E$11*100</f>
         <v>81.269841269841265</v>
       </c>
       <c r="H4" s="11" t="s">
@@ -671,7 +690,7 @@
         <v>334</v>
       </c>
       <c r="J4">
-        <f>I4/$I$11*100</f>
+        <f t="shared" ref="J4:J11" si="1">I4/$I$11*100</f>
         <v>71.215351812366734</v>
       </c>
       <c r="L4" s="11" t="s">
@@ -698,7 +717,7 @@
         <v>57</v>
       </c>
       <c r="F5">
-        <f>E5/$E$11*100</f>
+        <f t="shared" si="0"/>
         <v>9.0476190476190474</v>
       </c>
       <c r="H5" s="11" t="s">
@@ -708,7 +727,7 @@
         <v>48</v>
       </c>
       <c r="J5">
-        <f>I5/$I$11*100</f>
+        <f t="shared" si="1"/>
         <v>10.23454157782516</v>
       </c>
     </row>
@@ -726,7 +745,7 @@
         <v>25</v>
       </c>
       <c r="F6">
-        <f>E6/$E$11*100</f>
+        <f t="shared" si="0"/>
         <v>3.9682539682539679</v>
       </c>
       <c r="H6" s="11" t="s">
@@ -736,7 +755,7 @@
         <v>48</v>
       </c>
       <c r="J6">
-        <f>I6/$I$11*100</f>
+        <f t="shared" si="1"/>
         <v>10.23454157782516</v>
       </c>
     </row>
@@ -754,7 +773,7 @@
         <v>25</v>
       </c>
       <c r="F7">
-        <f>E7/$E$11*100</f>
+        <f t="shared" si="0"/>
         <v>3.9682539682539679</v>
       </c>
       <c r="H7" s="11" t="s">
@@ -764,7 +783,7 @@
         <v>32</v>
       </c>
       <c r="J7">
-        <f>I7/$I$11*100</f>
+        <f t="shared" si="1"/>
         <v>6.8230277185501063</v>
       </c>
     </row>
@@ -782,7 +801,7 @@
         <v>9</v>
       </c>
       <c r="F8">
-        <f>E8/$E$11*100</f>
+        <f t="shared" si="0"/>
         <v>1.4285714285714286</v>
       </c>
       <c r="H8" s="11" t="s">
@@ -792,11 +811,15 @@
         <v>3</v>
       </c>
       <c r="J8">
-        <f>I8/$I$11*100</f>
+        <f t="shared" si="1"/>
         <v>0.63965884861407252</v>
       </c>
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="B9" s="4">
+        <f>SUM(B4:B8)</f>
+        <v>1457</v>
+      </c>
       <c r="D9" s="11" t="s">
         <v>13</v>
       </c>
@@ -804,7 +827,7 @@
         <v>1</v>
       </c>
       <c r="F9">
-        <f>E9/$E$11*100</f>
+        <f t="shared" si="0"/>
         <v>0.15873015873015872</v>
       </c>
       <c r="H9" s="11" t="s">
@@ -814,8 +837,17 @@
         <v>3</v>
       </c>
       <c r="J9">
-        <f>I9/$I$11*100</f>
+        <f t="shared" si="1"/>
         <v>0.63965884861407252</v>
+      </c>
+      <c r="L9" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="M9" s="17" t="s">
+        <v>7</v>
+      </c>
+      <c r="N9" s="16" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.3">
@@ -826,7 +858,7 @@
         <v>1</v>
       </c>
       <c r="F10">
-        <f>E10/$E$11*100</f>
+        <f t="shared" si="0"/>
         <v>0.15873015873015872</v>
       </c>
       <c r="H10" s="11" t="s">
@@ -836,8 +868,19 @@
         <v>1</v>
       </c>
       <c r="J10">
-        <f>I10/$I$11*100</f>
+        <f t="shared" si="1"/>
         <v>0.21321961620469082</v>
+      </c>
+      <c r="L10" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="M10">
+        <f>E4+I4+E15+I15+M4</f>
+        <v>1143</v>
+      </c>
+      <c r="N10">
+        <f>M10/1457*100</f>
+        <v>78.448867536032935</v>
       </c>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.3">
@@ -846,7 +889,7 @@
         <v>630</v>
       </c>
       <c r="F11">
-        <f>E11/$E$11*100</f>
+        <f t="shared" si="0"/>
         <v>100</v>
       </c>
       <c r="I11" s="4">
@@ -854,8 +897,45 @@
         <v>469</v>
       </c>
       <c r="J11">
-        <f>I11/$I$11*100</f>
+        <f t="shared" si="1"/>
         <v>100</v>
+      </c>
+      <c r="L11" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="M11">
+        <f>E5+I5+E17</f>
+        <v>111</v>
+      </c>
+      <c r="N11">
+        <f t="shared" ref="N11:N18" si="2">M11/1457*100</f>
+        <v>7.6183939601921757</v>
+      </c>
+    </row>
+    <row r="12" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="L12" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="M12">
+        <f>E6+I7+E18+I17</f>
+        <v>62</v>
+      </c>
+      <c r="N12">
+        <f t="shared" si="2"/>
+        <v>4.2553191489361701</v>
+      </c>
+    </row>
+    <row r="13" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="L13" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="M13">
+        <f>E7+I6+E16+I16</f>
+        <v>119</v>
+      </c>
+      <c r="N13">
+        <f t="shared" si="2"/>
+        <v>8.1674673987645843</v>
       </c>
     </row>
     <row r="14" spans="1:19" x14ac:dyDescent="0.3">
@@ -878,6 +958,17 @@
       <c r="J14" s="9" t="s">
         <v>16</v>
       </c>
+      <c r="L14" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="M14">
+        <f>E8+I8+E19+I18</f>
+        <v>14</v>
+      </c>
+      <c r="N14">
+        <f t="shared" si="2"/>
+        <v>0.96087851750171582</v>
+      </c>
     </row>
     <row r="15" spans="1:19" x14ac:dyDescent="0.3">
       <c r="D15" s="11" t="s">
@@ -887,7 +978,7 @@
         <v>246</v>
       </c>
       <c r="F15">
-        <f>E15/$E$22*100</f>
+        <f t="shared" ref="F15:F22" si="3">E15/$E$22*100</f>
         <v>82.550335570469798</v>
       </c>
       <c r="H15" s="11" t="s">
@@ -900,6 +991,17 @@
         <f>I15/$I$19*100</f>
         <v>84.210526315789465</v>
       </c>
+      <c r="L15" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="M15">
+        <f>E9+I9+E21</f>
+        <v>5</v>
+      </c>
+      <c r="N15">
+        <f t="shared" si="2"/>
+        <v>0.34317089910775567</v>
+      </c>
     </row>
     <row r="16" spans="1:19" x14ac:dyDescent="0.3">
       <c r="D16" s="11" t="s">
@@ -909,7 +1011,7 @@
         <v>41</v>
       </c>
       <c r="F16">
-        <f>E16/$E$22*100</f>
+        <f t="shared" si="3"/>
         <v>13.758389261744966</v>
       </c>
       <c r="H16" s="11" t="s">
@@ -922,8 +1024,19 @@
         <f>I16/$I$19*100</f>
         <v>8.7719298245614024</v>
       </c>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="L16" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="M16">
+        <f>E10</f>
+        <v>1</v>
+      </c>
+      <c r="N16">
+        <f t="shared" si="2"/>
+        <v>6.8634179821551136E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.3">
       <c r="D17" s="11" t="s">
         <v>9</v>
       </c>
@@ -931,7 +1044,7 @@
         <v>6</v>
       </c>
       <c r="F17">
-        <f>E17/$E$22*100</f>
+        <f t="shared" si="3"/>
         <v>2.0134228187919461</v>
       </c>
       <c r="H17" s="11" t="s">
@@ -944,8 +1057,19 @@
         <f>I17/$I$19*100</f>
         <v>5.2631578947368416</v>
       </c>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="L17" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="M17" s="4">
+        <f>I10+E20</f>
+        <v>2</v>
+      </c>
+      <c r="N17">
+        <f t="shared" si="2"/>
+        <v>0.13726835964310227</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.3">
       <c r="D18" s="11" t="s">
         <v>10</v>
       </c>
@@ -953,7 +1077,7 @@
         <v>2</v>
       </c>
       <c r="F18">
-        <f>E18/$E$22*100</f>
+        <f t="shared" si="3"/>
         <v>0.67114093959731547</v>
       </c>
       <c r="H18" s="11" t="s">
@@ -966,8 +1090,16 @@
         <f>I18/$I$19*100</f>
         <v>1.7543859649122806</v>
       </c>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="M18" s="4">
+        <f>SUM(M10:M17)</f>
+        <v>1457</v>
+      </c>
+      <c r="N18">
+        <f t="shared" si="2"/>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.3">
       <c r="D19" s="11" t="s">
         <v>12</v>
       </c>
@@ -975,7 +1107,7 @@
         <v>1</v>
       </c>
       <c r="F19">
-        <f>E19/$E$22*100</f>
+        <f t="shared" si="3"/>
         <v>0.33557046979865773</v>
       </c>
       <c r="I19" s="4">
@@ -987,7 +1119,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:14" x14ac:dyDescent="0.3">
       <c r="D20" s="11" t="s">
         <v>15</v>
       </c>
@@ -995,11 +1127,11 @@
         <v>1</v>
       </c>
       <c r="F20">
-        <f>E20/$E$22*100</f>
+        <f t="shared" si="3"/>
         <v>0.33557046979865773</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:14" x14ac:dyDescent="0.3">
       <c r="D21" s="11" t="s">
         <v>13</v>
       </c>
@@ -1007,27 +1139,27 @@
         <v>1</v>
       </c>
       <c r="F21">
-        <f>E21/$E$22*100</f>
+        <f t="shared" si="3"/>
         <v>0.33557046979865773</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:14" x14ac:dyDescent="0.3">
       <c r="E22" s="4">
         <f>SUM(E15:E21)</f>
         <v>298</v>
       </c>
       <c r="F22">
-        <f>E22/$E$22*100</f>
+        <f t="shared" si="3"/>
         <v>100</v>
       </c>
     </row>
-    <row r="24" spans="1:10" s="12" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="25" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:14" s="12" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="25" spans="1:14" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A25" s="2" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B27" s="3" t="s">
         <v>0</v>
       </c>
@@ -1049,8 +1181,17 @@
       <c r="J27" s="10" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="L27" s="16" t="s">
+        <v>26</v>
+      </c>
+      <c r="M27" s="16" t="s">
+        <v>7</v>
+      </c>
+      <c r="N27" s="16" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="28" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A28" s="3" t="s">
         <v>5</v>
       </c>
@@ -1077,8 +1218,19 @@
         <f>I28/$I$34*100</f>
         <v>66.984126984126974</v>
       </c>
-    </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="L28" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="M28">
+        <f>E28+I28+E41+I41</f>
+        <v>689</v>
+      </c>
+      <c r="N28">
+        <f>M28/1038*100</f>
+        <v>66.377649325626209</v>
+      </c>
+    </row>
+    <row r="29" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A29" s="3" t="s">
         <v>17</v>
       </c>
@@ -1092,7 +1244,7 @@
         <v>129</v>
       </c>
       <c r="F29">
-        <f t="shared" ref="F29:F36" si="0">E29/$E$37*100</f>
+        <f t="shared" ref="F29:F36" si="4">E29/$E$37*100</f>
         <v>18.041958041958043</v>
       </c>
       <c r="H29" s="11" t="s">
@@ -1102,11 +1254,22 @@
         <v>57</v>
       </c>
       <c r="J29">
-        <f t="shared" ref="J29:J34" si="1">I29/$I$34*100</f>
+        <f t="shared" ref="J29:J34" si="5">I29/$I$34*100</f>
         <v>18.095238095238095</v>
       </c>
-    </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="L29" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="M29">
+        <f>E29+I29</f>
+        <v>186</v>
+      </c>
+      <c r="N29">
+        <f t="shared" ref="N29:N37" si="6">M29/1038*100</f>
+        <v>17.919075144508671</v>
+      </c>
+    </row>
+    <row r="30" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A30" s="3" t="s">
         <v>1</v>
       </c>
@@ -1120,7 +1283,7 @@
         <v>65</v>
       </c>
       <c r="F30">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>9.0909090909090917</v>
       </c>
       <c r="H30" s="11" t="s">
@@ -1130,11 +1293,22 @@
         <v>28</v>
       </c>
       <c r="J30">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>8.8888888888888893</v>
       </c>
-    </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="L30" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="M30">
+        <f>E30+I30+E42</f>
+        <v>94</v>
+      </c>
+      <c r="N30">
+        <f t="shared" si="6"/>
+        <v>9.0558766859344892</v>
+      </c>
+    </row>
+    <row r="31" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A31" s="3" t="s">
         <v>2</v>
       </c>
@@ -1148,7 +1322,7 @@
         <v>38</v>
       </c>
       <c r="F31">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>5.314685314685315</v>
       </c>
       <c r="H31" s="11" t="s">
@@ -1158,11 +1332,26 @@
         <v>10</v>
       </c>
       <c r="J31">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>3.1746031746031744</v>
       </c>
-    </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="L31" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="M31">
+        <f>E31+I31</f>
+        <v>48</v>
+      </c>
+      <c r="N31">
+        <f t="shared" si="6"/>
+        <v>4.6242774566473983</v>
+      </c>
+    </row>
+    <row r="32" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="B32" s="4">
+        <f>SUM(B28:B31)</f>
+        <v>1038</v>
+      </c>
       <c r="D32" s="11" t="s">
         <v>12</v>
       </c>
@@ -1170,7 +1359,7 @@
         <v>5</v>
       </c>
       <c r="F32">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>0.69930069930069927</v>
       </c>
       <c r="H32" s="11" t="s">
@@ -1180,11 +1369,22 @@
         <v>6</v>
       </c>
       <c r="J32">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>1.9047619047619049</v>
       </c>
-    </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="L32" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="M32">
+        <f>E32+I33</f>
+        <v>8</v>
+      </c>
+      <c r="N32">
+        <f t="shared" si="6"/>
+        <v>0.77071290944123316</v>
+      </c>
+    </row>
+    <row r="33" spans="1:14" x14ac:dyDescent="0.3">
       <c r="D33" s="11" t="s">
         <v>13</v>
       </c>
@@ -1192,7 +1392,7 @@
         <v>3</v>
       </c>
       <c r="F33">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>0.41958041958041958</v>
       </c>
       <c r="H33" s="11" t="s">
@@ -1202,11 +1402,22 @@
         <v>3</v>
       </c>
       <c r="J33">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>0.95238095238095244</v>
       </c>
-    </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="L33" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="M33">
+        <f>E33+I32</f>
+        <v>9</v>
+      </c>
+      <c r="N33">
+        <f t="shared" si="6"/>
+        <v>0.86705202312138718</v>
+      </c>
+    </row>
+    <row r="34" spans="1:14" x14ac:dyDescent="0.3">
       <c r="D34" s="11" t="s">
         <v>15</v>
       </c>
@@ -1214,7 +1425,7 @@
         <v>2</v>
       </c>
       <c r="F34">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>0.27972027972027974</v>
       </c>
       <c r="I34" s="4">
@@ -1222,11 +1433,22 @@
         <v>315</v>
       </c>
       <c r="J34">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>100</v>
       </c>
-    </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="L34" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="M34">
+        <f>E34</f>
+        <v>2</v>
+      </c>
+      <c r="N34">
+        <f t="shared" si="6"/>
+        <v>0.19267822736030829</v>
+      </c>
+    </row>
+    <row r="35" spans="1:14" x14ac:dyDescent="0.3">
       <c r="D35" s="11" t="s">
         <v>19</v>
       </c>
@@ -1234,11 +1456,22 @@
         <v>1</v>
       </c>
       <c r="F35">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>0.13986013986013987</v>
       </c>
-    </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="L35" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="M35">
+        <f t="shared" ref="M35:M36" si="7">E35</f>
+        <v>1</v>
+      </c>
+      <c r="N35">
+        <f t="shared" si="6"/>
+        <v>9.6339113680154145E-2</v>
+      </c>
+    </row>
+    <row r="36" spans="1:14" x14ac:dyDescent="0.3">
       <c r="D36" s="11" t="s">
         <v>20</v>
       </c>
@@ -1246,11 +1479,22 @@
         <v>1</v>
       </c>
       <c r="F36">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>0.13986013986013987</v>
       </c>
-    </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="L36" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="M36">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="N36">
+        <f t="shared" si="6"/>
+        <v>9.6339113680154145E-2</v>
+      </c>
+    </row>
+    <row r="37" spans="1:14" x14ac:dyDescent="0.3">
       <c r="E37" s="4">
         <f>SUM(E28:E36)</f>
         <v>715</v>
@@ -1259,8 +1503,16 @@
         <f>E37/$E$37*100</f>
         <v>100</v>
       </c>
-    </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="M37" s="4">
+        <f>SUM(M28:M36)</f>
+        <v>1038</v>
+      </c>
+      <c r="N37">
+        <f t="shared" si="6"/>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="40" spans="1:14" x14ac:dyDescent="0.3">
       <c r="D40" s="6" t="s">
         <v>1</v>
       </c>
@@ -1280,7 +1532,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:14" x14ac:dyDescent="0.3">
       <c r="D41" s="11" t="s">
         <v>8</v>
       </c>
@@ -1301,7 +1553,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:14" x14ac:dyDescent="0.3">
       <c r="D42" s="11" t="s">
         <v>10</v>
       </c>
@@ -1313,19 +1565,19 @@
         <v>14.285714285714285</v>
       </c>
     </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:14" x14ac:dyDescent="0.3">
       <c r="E43" s="4">
         <f>SUM(E41:E42)</f>
         <v>7</v>
       </c>
     </row>
-    <row r="45" spans="1:10" s="12" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="46" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:14" s="12" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="46" spans="1:14" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A46" s="2" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B48" s="3" t="s">
         <v>0</v>
       </c>
@@ -1347,8 +1599,17 @@
       <c r="J48" s="10" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="L48" s="16" t="s">
+        <v>27</v>
+      </c>
+      <c r="M48" s="16" t="s">
+        <v>7</v>
+      </c>
+      <c r="N48" s="16" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="49" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A49" s="3" t="s">
         <v>5</v>
       </c>
@@ -1375,8 +1636,19 @@
         <f>I49/$I$54*100</f>
         <v>76.767676767676761</v>
       </c>
-    </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="L49" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="M49">
+        <f>E62+I62+I49+E49</f>
+        <v>751</v>
+      </c>
+      <c r="N49">
+        <f>M49/1109*100</f>
+        <v>67.718665464382326</v>
+      </c>
+    </row>
+    <row r="50" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A50" s="3" t="s">
         <v>1</v>
       </c>
@@ -1390,7 +1662,7 @@
         <v>168</v>
       </c>
       <c r="F50">
-        <f t="shared" ref="F50:F59" si="2">E50/$E$59*100</f>
+        <f t="shared" ref="F50:F59" si="8">E50/$E$59*100</f>
         <v>16.766467065868262</v>
       </c>
       <c r="H50" s="11" t="s">
@@ -1400,11 +1672,22 @@
         <v>9</v>
       </c>
       <c r="J50">
-        <f t="shared" ref="J50:J54" si="3">I50/$I$54*100</f>
+        <f t="shared" ref="J50:J54" si="9">I50/$I$54*100</f>
         <v>9.0909090909090917</v>
       </c>
-    </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="L50" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="M50">
+        <f>E50+I51+E63</f>
+        <v>177</v>
+      </c>
+      <c r="N50">
+        <f t="shared" ref="N50:N59" si="10">M50/1109*100</f>
+        <v>15.960324616771867</v>
+      </c>
+    </row>
+    <row r="51" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A51" s="3" t="s">
         <v>17</v>
       </c>
@@ -1418,7 +1701,7 @@
         <v>94</v>
       </c>
       <c r="F51">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>9.3812375249500999</v>
       </c>
       <c r="H51" s="11" t="s">
@@ -1428,11 +1711,22 @@
         <v>8</v>
       </c>
       <c r="J51">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>8.0808080808080813</v>
       </c>
-    </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="L51" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="M51">
+        <f>E51+I50</f>
+        <v>103</v>
+      </c>
+      <c r="N51">
+        <f t="shared" si="10"/>
+        <v>9.2876465284039664</v>
+      </c>
+    </row>
+    <row r="52" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A52" s="3" t="s">
         <v>2</v>
       </c>
@@ -1446,7 +1740,7 @@
         <v>56</v>
       </c>
       <c r="F52">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>5.5888223552894214</v>
       </c>
       <c r="H52" s="11" t="s">
@@ -1456,11 +1750,26 @@
         <v>5</v>
       </c>
       <c r="J52">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>5.0505050505050502</v>
       </c>
-    </row>
-    <row r="53" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="L52" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="M52">
+        <f>E52+I52</f>
+        <v>61</v>
+      </c>
+      <c r="N52">
+        <f t="shared" si="10"/>
+        <v>5.5004508566275927</v>
+      </c>
+    </row>
+    <row r="53" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="B53" s="4">
+        <f>SUM(B49:B52)</f>
+        <v>1109</v>
+      </c>
       <c r="D53" s="11" t="s">
         <v>13</v>
       </c>
@@ -1468,7 +1777,7 @@
         <v>7</v>
       </c>
       <c r="F53">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>0.69860279441117767</v>
       </c>
       <c r="H53" s="11" t="s">
@@ -1478,11 +1787,22 @@
         <v>1</v>
       </c>
       <c r="J53">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>1.0101010101010102</v>
       </c>
-    </row>
-    <row r="54" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="L53" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="M53">
+        <f>E53</f>
+        <v>7</v>
+      </c>
+      <c r="N53">
+        <f t="shared" si="10"/>
+        <v>0.63119927862939584</v>
+      </c>
+    </row>
+    <row r="54" spans="1:14" x14ac:dyDescent="0.3">
       <c r="D54" s="11" t="s">
         <v>12</v>
       </c>
@@ -1490,7 +1810,7 @@
         <v>3</v>
       </c>
       <c r="F54">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>0.29940119760479045</v>
       </c>
       <c r="I54" s="4">
@@ -1498,11 +1818,22 @@
         <v>99</v>
       </c>
       <c r="J54">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>100</v>
       </c>
-    </row>
-    <row r="55" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="L54" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="M54">
+        <f>E54+I53</f>
+        <v>4</v>
+      </c>
+      <c r="N54">
+        <f t="shared" si="10"/>
+        <v>0.36068530207394045</v>
+      </c>
+    </row>
+    <row r="55" spans="1:14" x14ac:dyDescent="0.3">
       <c r="D55" s="11" t="s">
         <v>14</v>
       </c>
@@ -1510,11 +1841,22 @@
         <v>2</v>
       </c>
       <c r="F55">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>0.19960079840319359</v>
       </c>
-    </row>
-    <row r="56" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="L55" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="M55">
+        <f>E55</f>
+        <v>2</v>
+      </c>
+      <c r="N55">
+        <f t="shared" si="10"/>
+        <v>0.18034265103697023</v>
+      </c>
+    </row>
+    <row r="56" spans="1:14" x14ac:dyDescent="0.3">
       <c r="D56" s="11" t="s">
         <v>20</v>
       </c>
@@ -1522,11 +1864,22 @@
         <v>2</v>
       </c>
       <c r="F56">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>0.19960079840319359</v>
       </c>
-    </row>
-    <row r="57" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="L56" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="M56">
+        <f t="shared" ref="M56:M58" si="11">E56</f>
+        <v>2</v>
+      </c>
+      <c r="N56">
+        <f t="shared" si="10"/>
+        <v>0.18034265103697023</v>
+      </c>
+    </row>
+    <row r="57" spans="1:14" x14ac:dyDescent="0.3">
       <c r="D57" s="11" t="s">
         <v>19</v>
       </c>
@@ -1534,11 +1887,22 @@
         <v>1</v>
       </c>
       <c r="F57">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>9.9800399201596793E-2</v>
       </c>
-    </row>
-    <row r="58" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="L57" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="M57">
+        <f t="shared" si="11"/>
+        <v>1</v>
+      </c>
+      <c r="N57">
+        <f t="shared" si="10"/>
+        <v>9.0171325518485113E-2</v>
+      </c>
+    </row>
+    <row r="58" spans="1:14" x14ac:dyDescent="0.3">
       <c r="D58" s="11" t="s">
         <v>15</v>
       </c>
@@ -1546,21 +1910,40 @@
         <v>1</v>
       </c>
       <c r="F58">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>9.9800399201596793E-2</v>
       </c>
-    </row>
-    <row r="59" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="L58" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="M58">
+        <f t="shared" si="11"/>
+        <v>1</v>
+      </c>
+      <c r="N58">
+        <f t="shared" si="10"/>
+        <v>9.0171325518485113E-2</v>
+      </c>
+    </row>
+    <row r="59" spans="1:14" x14ac:dyDescent="0.3">
       <c r="E59" s="4">
         <f>SUM(E49:E58)</f>
         <v>1002</v>
       </c>
       <c r="F59">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>100</v>
       </c>
-    </row>
-    <row r="61" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="M59" s="4">
+        <f>SUM(M49:M58)</f>
+        <v>1109</v>
+      </c>
+      <c r="N59">
+        <f t="shared" si="10"/>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="61" spans="1:14" x14ac:dyDescent="0.3">
       <c r="D61" s="8" t="s">
         <v>17</v>
       </c>
@@ -1580,7 +1963,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="62" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:14" x14ac:dyDescent="0.3">
       <c r="D62" s="11" t="s">
         <v>8</v>
       </c>
@@ -1601,7 +1984,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="63" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:14" x14ac:dyDescent="0.3">
       <c r="D63" s="11" t="s">
         <v>9</v>
       </c>
@@ -1613,7 +1996,7 @@
         <v>14.285714285714285</v>
       </c>
     </row>
-    <row r="64" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:14" x14ac:dyDescent="0.3">
       <c r="E64" s="4">
         <f>SUM(E62:E63)</f>
         <v>7</v>
@@ -1623,13 +2006,13 @@
         <v>100</v>
       </c>
     </row>
-    <row r="66" spans="1:10" s="15" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="67" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:14" s="15" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="67" spans="1:14" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A67" s="2" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="69" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B69" s="3" t="s">
         <v>0</v>
       </c>
@@ -1651,8 +2034,17 @@
       <c r="J69" s="10" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="70" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="L69" s="16" t="s">
+        <v>28</v>
+      </c>
+      <c r="M69" s="16" t="s">
+        <v>7</v>
+      </c>
+      <c r="N69" s="16" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="70" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A70" s="3" t="s">
         <v>5</v>
       </c>
@@ -1679,8 +2071,19 @@
         <f>I70/$I$75*100</f>
         <v>60</v>
       </c>
-    </row>
-    <row r="71" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="L70" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="M70">
+        <f>E70+I70+E82</f>
+        <v>239</v>
+      </c>
+      <c r="N70">
+        <f>M70/466*100</f>
+        <v>51.287553648068673</v>
+      </c>
+    </row>
+    <row r="71" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A71" s="3" t="s">
         <v>4</v>
       </c>
@@ -1694,7 +2097,7 @@
         <v>126</v>
       </c>
       <c r="F71">
-        <f t="shared" ref="F71:F79" si="4">E71/$E$79*100</f>
+        <f t="shared" ref="F71:F79" si="12">E71/$E$79*100</f>
         <v>28.187919463087248</v>
       </c>
       <c r="H71" s="11" t="s">
@@ -1704,11 +2107,22 @@
         <v>3</v>
       </c>
       <c r="J71">
-        <f t="shared" ref="J71:J75" si="5">I71/$I$75*100</f>
+        <f t="shared" ref="J71:J75" si="13">I71/$I$75*100</f>
         <v>20</v>
       </c>
-    </row>
-    <row r="72" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="L71" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="M71">
+        <f>E71+I82+I72</f>
+        <v>128</v>
+      </c>
+      <c r="N71">
+        <f t="shared" ref="N71:N79" si="14">M71/466*100</f>
+        <v>27.467811158798284</v>
+      </c>
+    </row>
+    <row r="72" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A72" s="3" t="s">
         <v>17</v>
       </c>
@@ -1722,7 +2136,7 @@
         <v>52</v>
       </c>
       <c r="F72">
-        <f t="shared" si="4"/>
+        <f t="shared" si="12"/>
         <v>11.633109619686801</v>
       </c>
       <c r="H72" s="11" t="s">
@@ -1732,11 +2146,22 @@
         <v>1</v>
       </c>
       <c r="J72">
-        <f t="shared" si="5"/>
+        <f t="shared" si="13"/>
         <v>6.666666666666667</v>
       </c>
-    </row>
-    <row r="73" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="L72" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="M72">
+        <f>E72+I73</f>
+        <v>53</v>
+      </c>
+      <c r="N72">
+        <f t="shared" si="14"/>
+        <v>11.373390557939913</v>
+      </c>
+    </row>
+    <row r="73" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A73" s="3" t="s">
         <v>1</v>
       </c>
@@ -1750,7 +2175,7 @@
         <v>22</v>
       </c>
       <c r="F73">
-        <f t="shared" si="4"/>
+        <f t="shared" si="12"/>
         <v>4.9217002237136462</v>
       </c>
       <c r="H73" s="11" t="s">
@@ -1760,11 +2185,26 @@
         <v>1</v>
       </c>
       <c r="J73">
-        <f t="shared" si="5"/>
+        <f t="shared" si="13"/>
         <v>6.666666666666667</v>
       </c>
-    </row>
-    <row r="74" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="L73" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="M73">
+        <f>E73+E83</f>
+        <v>23</v>
+      </c>
+      <c r="N73">
+        <f t="shared" si="14"/>
+        <v>4.9356223175965663</v>
+      </c>
+    </row>
+    <row r="74" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="B74" s="4">
+        <f>SUM(B70:B73)</f>
+        <v>466</v>
+      </c>
       <c r="D74" s="11" t="s">
         <v>13</v>
       </c>
@@ -1772,7 +2212,7 @@
         <v>6</v>
       </c>
       <c r="F74">
-        <f t="shared" si="4"/>
+        <f t="shared" si="12"/>
         <v>1.3422818791946309</v>
       </c>
       <c r="H74" s="11" t="s">
@@ -1782,11 +2222,22 @@
         <v>1</v>
       </c>
       <c r="J74">
-        <f t="shared" si="5"/>
+        <f t="shared" si="13"/>
         <v>6.666666666666667</v>
       </c>
-    </row>
-    <row r="75" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="L74" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="M74">
+        <f>E74</f>
+        <v>6</v>
+      </c>
+      <c r="N74">
+        <f t="shared" si="14"/>
+        <v>1.2875536480686696</v>
+      </c>
+    </row>
+    <row r="75" spans="1:14" x14ac:dyDescent="0.3">
       <c r="D75" s="11" t="s">
         <v>20</v>
       </c>
@@ -1794,7 +2245,7 @@
         <v>6</v>
       </c>
       <c r="F75">
-        <f t="shared" si="4"/>
+        <f t="shared" si="12"/>
         <v>1.3422818791946309</v>
       </c>
       <c r="I75" s="4">
@@ -1802,11 +2253,22 @@
         <v>15</v>
       </c>
       <c r="J75">
-        <f t="shared" si="5"/>
+        <f t="shared" si="13"/>
         <v>100</v>
       </c>
-    </row>
-    <row r="76" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="L75" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="M75">
+        <f>E75+I71</f>
+        <v>9</v>
+      </c>
+      <c r="N75">
+        <f t="shared" si="14"/>
+        <v>1.9313304721030045</v>
+      </c>
+    </row>
+    <row r="76" spans="1:14" x14ac:dyDescent="0.3">
       <c r="D76" s="11" t="s">
         <v>12</v>
       </c>
@@ -1814,11 +2276,22 @@
         <v>4</v>
       </c>
       <c r="F76">
-        <f t="shared" si="4"/>
+        <f t="shared" si="12"/>
         <v>0.89485458612975388</v>
       </c>
-    </row>
-    <row r="77" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="L76" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="M76">
+        <f>E76+I74</f>
+        <v>5</v>
+      </c>
+      <c r="N76">
+        <f t="shared" si="14"/>
+        <v>1.0729613733905579</v>
+      </c>
+    </row>
+    <row r="77" spans="1:14" x14ac:dyDescent="0.3">
       <c r="D77" s="11" t="s">
         <v>19</v>
       </c>
@@ -1826,11 +2299,22 @@
         <v>2</v>
       </c>
       <c r="F77">
-        <f t="shared" si="4"/>
+        <f t="shared" si="12"/>
         <v>0.44742729306487694</v>
       </c>
-    </row>
-    <row r="78" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="L77" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="M77">
+        <f>E77</f>
+        <v>2</v>
+      </c>
+      <c r="N77">
+        <f t="shared" si="14"/>
+        <v>0.42918454935622319</v>
+      </c>
+    </row>
+    <row r="78" spans="1:14" x14ac:dyDescent="0.3">
       <c r="D78" s="11" t="s">
         <v>23</v>
       </c>
@@ -1838,21 +2322,40 @@
         <v>1</v>
       </c>
       <c r="F78">
-        <f t="shared" si="4"/>
+        <f t="shared" si="12"/>
         <v>0.22371364653243847</v>
       </c>
-    </row>
-    <row r="79" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="L78" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="M78">
+        <f>E78</f>
+        <v>1</v>
+      </c>
+      <c r="N78">
+        <f t="shared" si="14"/>
+        <v>0.21459227467811159</v>
+      </c>
+    </row>
+    <row r="79" spans="1:14" x14ac:dyDescent="0.3">
       <c r="E79" s="4">
         <f>SUM(E70:E78)</f>
         <v>447</v>
       </c>
       <c r="F79">
-        <f t="shared" si="4"/>
+        <f t="shared" si="12"/>
         <v>100</v>
       </c>
-    </row>
-    <row r="81" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="M79" s="4">
+        <f>SUM(M70:M78)</f>
+        <v>466</v>
+      </c>
+      <c r="N79">
+        <f t="shared" si="14"/>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="81" spans="1:14" x14ac:dyDescent="0.3">
       <c r="D81" s="8" t="s">
         <v>17</v>
       </c>
@@ -1872,7 +2375,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="82" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:14" x14ac:dyDescent="0.3">
       <c r="D82" s="11" t="s">
         <v>8</v>
       </c>
@@ -1892,7 +2395,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="83" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:14" x14ac:dyDescent="0.3">
       <c r="D83" s="11" t="s">
         <v>11</v>
       </c>
@@ -1903,7 +2406,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="84" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:14" x14ac:dyDescent="0.3">
       <c r="E84" s="4">
         <f>SUM(E82:E83)</f>
         <v>3</v>
@@ -1912,13 +2415,13 @@
         <v>100</v>
       </c>
     </row>
-    <row r="86" spans="1:10" s="15" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="87" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:14" s="15" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="87" spans="1:14" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A87" s="2" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="89" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B89" s="3" t="s">
         <v>0</v>
       </c>
@@ -1940,8 +2443,17 @@
       <c r="J89" s="10" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="90" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="L89" s="16" t="s">
+        <v>29</v>
+      </c>
+      <c r="M89" s="16" t="s">
+        <v>7</v>
+      </c>
+      <c r="N89" s="16" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="90" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A90" s="3" t="s">
         <v>5</v>
       </c>
@@ -1968,8 +2480,19 @@
         <f>I90/$I$94*100</f>
         <v>69.230769230769226</v>
       </c>
-    </row>
-    <row r="91" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="L90" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="M90">
+        <f>E90+I90+E99</f>
+        <v>144</v>
+      </c>
+      <c r="N90">
+        <f>M90/179*100</f>
+        <v>80.44692737430168</v>
+      </c>
+    </row>
+    <row r="91" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A91" s="3" t="s">
         <v>17</v>
       </c>
@@ -1983,7 +2506,7 @@
         <v>10</v>
       </c>
       <c r="F91">
-        <f t="shared" ref="F91:F96" si="6">E91/$E$96*100</f>
+        <f t="shared" ref="F91:F96" si="15">E91/$E$96*100</f>
         <v>6.0975609756097562</v>
       </c>
       <c r="H91" s="11" t="s">
@@ -1993,11 +2516,22 @@
         <v>2</v>
       </c>
       <c r="J91">
-        <f t="shared" ref="J91:J94" si="7">I91/$I$94*100</f>
+        <f t="shared" ref="J91:J94" si="16">I91/$I$94*100</f>
         <v>15.384615384615385</v>
       </c>
-    </row>
-    <row r="92" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="L91" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="M91">
+        <f>E91</f>
+        <v>10</v>
+      </c>
+      <c r="N91">
+        <f t="shared" ref="N91:N96" si="17">M91/179*100</f>
+        <v>5.5865921787709496</v>
+      </c>
+    </row>
+    <row r="92" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A92" s="3" t="s">
         <v>4</v>
       </c>
@@ -2011,7 +2545,7 @@
         <v>9</v>
       </c>
       <c r="F92">
-        <f t="shared" si="6"/>
+        <f t="shared" si="15"/>
         <v>5.4878048780487809</v>
       </c>
       <c r="H92" s="11" t="s">
@@ -2021,11 +2555,26 @@
         <v>1</v>
       </c>
       <c r="J92">
-        <f t="shared" si="7"/>
+        <f t="shared" si="16"/>
         <v>7.6923076923076925</v>
       </c>
-    </row>
-    <row r="93" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="L92" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="M92">
+        <f>E92+I92</f>
+        <v>10</v>
+      </c>
+      <c r="N92">
+        <f t="shared" si="17"/>
+        <v>5.5865921787709496</v>
+      </c>
+    </row>
+    <row r="93" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="B93" s="4">
+        <f>SUM(B90:B92)</f>
+        <v>179</v>
+      </c>
       <c r="D93" s="11" t="s">
         <v>9</v>
       </c>
@@ -2033,7 +2582,7 @@
         <v>9</v>
       </c>
       <c r="F93">
-        <f t="shared" si="6"/>
+        <f t="shared" si="15"/>
         <v>5.4878048780487809</v>
       </c>
       <c r="H93" s="11" t="s">
@@ -2043,11 +2592,22 @@
         <v>1</v>
       </c>
       <c r="J93">
-        <f t="shared" si="7"/>
+        <f t="shared" si="16"/>
         <v>7.6923076923076925</v>
       </c>
-    </row>
-    <row r="94" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="L93" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="M93">
+        <f>E93+I91</f>
+        <v>11</v>
+      </c>
+      <c r="N93">
+        <f t="shared" si="17"/>
+        <v>6.1452513966480442</v>
+      </c>
+    </row>
+    <row r="94" spans="1:14" x14ac:dyDescent="0.3">
       <c r="D94" s="11" t="s">
         <v>15</v>
       </c>
@@ -2055,7 +2615,7 @@
         <v>2</v>
       </c>
       <c r="F94">
-        <f t="shared" si="6"/>
+        <f t="shared" si="15"/>
         <v>1.2195121951219512</v>
       </c>
       <c r="I94" s="4">
@@ -2063,11 +2623,22 @@
         <v>13</v>
       </c>
       <c r="J94">
-        <f t="shared" si="7"/>
+        <f t="shared" si="16"/>
         <v>100</v>
       </c>
-    </row>
-    <row r="95" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="L94" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="M94">
+        <f>E94</f>
+        <v>2</v>
+      </c>
+      <c r="N94">
+        <f t="shared" si="17"/>
+        <v>1.1173184357541899</v>
+      </c>
+    </row>
+    <row r="95" spans="1:14" x14ac:dyDescent="0.3">
       <c r="D95" s="11" t="s">
         <v>13</v>
       </c>
@@ -2075,21 +2646,40 @@
         <v>1</v>
       </c>
       <c r="F95">
-        <f t="shared" si="6"/>
+        <f t="shared" si="15"/>
         <v>0.6097560975609756</v>
       </c>
-    </row>
-    <row r="96" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="L95" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="M95">
+        <f>E95+I93</f>
+        <v>2</v>
+      </c>
+      <c r="N95">
+        <f t="shared" si="17"/>
+        <v>1.1173184357541899</v>
+      </c>
+    </row>
+    <row r="96" spans="1:14" x14ac:dyDescent="0.3">
       <c r="E96" s="4">
         <f>SUM(E90:E95)</f>
         <v>164</v>
       </c>
       <c r="F96">
-        <f t="shared" si="6"/>
+        <f t="shared" si="15"/>
         <v>100</v>
       </c>
-    </row>
-    <row r="98" spans="4:6" x14ac:dyDescent="0.3">
+      <c r="M96" s="4">
+        <f>SUM(M90:M95)</f>
+        <v>179</v>
+      </c>
+      <c r="N96">
+        <f t="shared" si="17"/>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="98" spans="4:14" x14ac:dyDescent="0.3">
       <c r="D98" s="8" t="s">
         <v>4</v>
       </c>
@@ -2100,7 +2690,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="99" spans="4:6" x14ac:dyDescent="0.3">
+    <row r="99" spans="4:14" x14ac:dyDescent="0.3">
       <c r="D99" s="11" t="s">
         <v>8</v>
       </c>
@@ -2108,6 +2698,507 @@
         <v>2</v>
       </c>
       <c r="F99">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="102" spans="4:14" s="15" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="104" spans="4:14" x14ac:dyDescent="0.3">
+      <c r="D104" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="E104" s="16" t="s">
+        <v>7</v>
+      </c>
+      <c r="F104" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="H104" s="16" t="s">
+        <v>26</v>
+      </c>
+      <c r="I104" s="16" t="s">
+        <v>7</v>
+      </c>
+      <c r="J104" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="L104" s="16" t="s">
+        <v>27</v>
+      </c>
+      <c r="M104" s="16" t="s">
+        <v>7</v>
+      </c>
+      <c r="N104" s="16" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="105" spans="4:14" x14ac:dyDescent="0.3">
+      <c r="D105" s="18" t="s">
+        <v>8</v>
+      </c>
+      <c r="E105">
+        <v>1143</v>
+      </c>
+      <c r="F105">
+        <v>78.448867536032935</v>
+      </c>
+      <c r="H105" s="18" t="s">
+        <v>8</v>
+      </c>
+      <c r="I105">
+        <v>689</v>
+      </c>
+      <c r="J105">
+        <v>66.377649325626209</v>
+      </c>
+      <c r="L105" s="18" t="s">
+        <v>8</v>
+      </c>
+      <c r="M105">
+        <v>751</v>
+      </c>
+      <c r="N105">
+        <v>67.718665464382326</v>
+      </c>
+    </row>
+    <row r="106" spans="4:14" x14ac:dyDescent="0.3">
+      <c r="D106" s="18" t="s">
+        <v>9</v>
+      </c>
+      <c r="E106">
+        <v>111</v>
+      </c>
+      <c r="F106">
+        <v>7.6183939601921757</v>
+      </c>
+      <c r="H106" s="18" t="s">
+        <v>9</v>
+      </c>
+      <c r="I106">
+        <v>186</v>
+      </c>
+      <c r="J106">
+        <v>17.919075144508671</v>
+      </c>
+      <c r="L106" s="18" t="s">
+        <v>9</v>
+      </c>
+      <c r="M106">
+        <v>177</v>
+      </c>
+      <c r="N106">
+        <v>15.960324616771867</v>
+      </c>
+    </row>
+    <row r="107" spans="4:14" x14ac:dyDescent="0.3">
+      <c r="D107" s="18" t="s">
+        <v>10</v>
+      </c>
+      <c r="E107">
+        <v>62</v>
+      </c>
+      <c r="F107">
+        <v>4.2553191489361701</v>
+      </c>
+      <c r="H107" s="18" t="s">
+        <v>10</v>
+      </c>
+      <c r="I107">
+        <v>94</v>
+      </c>
+      <c r="J107">
+        <v>9.0558766859344892</v>
+      </c>
+      <c r="L107" s="18" t="s">
+        <v>10</v>
+      </c>
+      <c r="M107">
+        <v>103</v>
+      </c>
+      <c r="N107">
+        <v>9.2876465284039664</v>
+      </c>
+    </row>
+    <row r="108" spans="4:14" x14ac:dyDescent="0.3">
+      <c r="D108" s="18" t="s">
+        <v>11</v>
+      </c>
+      <c r="E108">
+        <v>119</v>
+      </c>
+      <c r="F108">
+        <v>8.1674673987645843</v>
+      </c>
+      <c r="H108" s="18" t="s">
+        <v>11</v>
+      </c>
+      <c r="I108">
+        <v>48</v>
+      </c>
+      <c r="J108">
+        <v>4.6242774566473983</v>
+      </c>
+      <c r="L108" s="18" t="s">
+        <v>11</v>
+      </c>
+      <c r="M108">
+        <v>61</v>
+      </c>
+      <c r="N108">
+        <v>5.5004508566275927</v>
+      </c>
+    </row>
+    <row r="109" spans="4:14" x14ac:dyDescent="0.3">
+      <c r="D109" s="18" t="s">
+        <v>12</v>
+      </c>
+      <c r="E109">
+        <v>14</v>
+      </c>
+      <c r="F109">
+        <v>0.96087851750171582</v>
+      </c>
+      <c r="H109" s="18" t="s">
+        <v>12</v>
+      </c>
+      <c r="I109">
+        <v>8</v>
+      </c>
+      <c r="J109">
+        <v>0.77071290944123316</v>
+      </c>
+      <c r="L109" s="18" t="s">
+        <v>13</v>
+      </c>
+      <c r="M109">
+        <v>7</v>
+      </c>
+      <c r="N109">
+        <v>0.63119927862939584</v>
+      </c>
+    </row>
+    <row r="110" spans="4:14" x14ac:dyDescent="0.3">
+      <c r="D110" s="18" t="s">
+        <v>13</v>
+      </c>
+      <c r="E110">
+        <v>5</v>
+      </c>
+      <c r="F110">
+        <v>0.34317089910775567</v>
+      </c>
+      <c r="H110" s="18" t="s">
+        <v>13</v>
+      </c>
+      <c r="I110">
+        <v>9</v>
+      </c>
+      <c r="J110">
+        <v>0.86705202312138718</v>
+      </c>
+      <c r="L110" s="18" t="s">
+        <v>12</v>
+      </c>
+      <c r="M110">
+        <v>4</v>
+      </c>
+      <c r="N110">
+        <v>0.36068530207394045</v>
+      </c>
+    </row>
+    <row r="111" spans="4:14" x14ac:dyDescent="0.3">
+      <c r="D111" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="E111">
+        <v>1</v>
+      </c>
+      <c r="F111">
+        <v>6.8634179821551136E-2</v>
+      </c>
+      <c r="H111" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="I111">
+        <v>2</v>
+      </c>
+      <c r="J111">
+        <v>0.19267822736030829</v>
+      </c>
+      <c r="L111" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="M111">
+        <v>2</v>
+      </c>
+      <c r="N111">
+        <v>0.18034265103697023</v>
+      </c>
+    </row>
+    <row r="112" spans="4:14" x14ac:dyDescent="0.3">
+      <c r="D112" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="E112">
+        <v>2</v>
+      </c>
+      <c r="F112">
+        <v>0.13726835964310227</v>
+      </c>
+      <c r="H112" s="18" t="s">
+        <v>19</v>
+      </c>
+      <c r="I112">
+        <v>1</v>
+      </c>
+      <c r="J112">
+        <v>9.6339113680154145E-2</v>
+      </c>
+      <c r="L112" s="18" t="s">
+        <v>20</v>
+      </c>
+      <c r="M112">
+        <v>2</v>
+      </c>
+      <c r="N112">
+        <v>0.18034265103697023</v>
+      </c>
+    </row>
+    <row r="113" spans="4:14" x14ac:dyDescent="0.3">
+      <c r="E113">
+        <v>1457</v>
+      </c>
+      <c r="F113">
+        <v>100</v>
+      </c>
+      <c r="H113" s="18" t="s">
+        <v>20</v>
+      </c>
+      <c r="I113">
+        <v>1</v>
+      </c>
+      <c r="J113">
+        <v>9.6339113680154145E-2</v>
+      </c>
+      <c r="L113" s="18" t="s">
+        <v>19</v>
+      </c>
+      <c r="M113">
+        <v>1</v>
+      </c>
+      <c r="N113">
+        <v>9.0171325518485113E-2</v>
+      </c>
+    </row>
+    <row r="114" spans="4:14" x14ac:dyDescent="0.3">
+      <c r="I114">
+        <v>1038</v>
+      </c>
+      <c r="J114">
+        <v>100</v>
+      </c>
+      <c r="L114" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="M114">
+        <v>1</v>
+      </c>
+      <c r="N114">
+        <v>9.0171325518485113E-2</v>
+      </c>
+    </row>
+    <row r="115" spans="4:14" x14ac:dyDescent="0.3">
+      <c r="L115" s="19"/>
+      <c r="M115">
+        <v>1109</v>
+      </c>
+      <c r="N115">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="117" spans="4:14" x14ac:dyDescent="0.3">
+      <c r="D117" s="16" t="s">
+        <v>28</v>
+      </c>
+      <c r="E117" s="16" t="s">
+        <v>7</v>
+      </c>
+      <c r="F117" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="H117" s="16" t="s">
+        <v>29</v>
+      </c>
+      <c r="I117" s="16" t="s">
+        <v>7</v>
+      </c>
+      <c r="J117" s="16" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="118" spans="4:14" x14ac:dyDescent="0.3">
+      <c r="D118" s="18" t="s">
+        <v>8</v>
+      </c>
+      <c r="E118">
+        <v>239</v>
+      </c>
+      <c r="F118">
+        <v>51.287553648068673</v>
+      </c>
+      <c r="H118" s="18" t="s">
+        <v>8</v>
+      </c>
+      <c r="I118">
+        <v>144</v>
+      </c>
+      <c r="J118">
+        <v>80.44692737430168</v>
+      </c>
+    </row>
+    <row r="119" spans="4:14" x14ac:dyDescent="0.3">
+      <c r="D119" s="18" t="s">
+        <v>9</v>
+      </c>
+      <c r="E119">
+        <v>128</v>
+      </c>
+      <c r="F119">
+        <v>27.467811158798284</v>
+      </c>
+      <c r="H119" s="18" t="s">
+        <v>10</v>
+      </c>
+      <c r="I119">
+        <v>10</v>
+      </c>
+      <c r="J119">
+        <v>5.5865921787709496</v>
+      </c>
+    </row>
+    <row r="120" spans="4:14" x14ac:dyDescent="0.3">
+      <c r="D120" s="18" t="s">
+        <v>10</v>
+      </c>
+      <c r="E120">
+        <v>53</v>
+      </c>
+      <c r="F120">
+        <v>11.373390557939913</v>
+      </c>
+      <c r="H120" s="18" t="s">
+        <v>11</v>
+      </c>
+      <c r="I120">
+        <v>10</v>
+      </c>
+      <c r="J120">
+        <v>5.5865921787709496</v>
+      </c>
+    </row>
+    <row r="121" spans="4:14" x14ac:dyDescent="0.3">
+      <c r="D121" s="18" t="s">
+        <v>11</v>
+      </c>
+      <c r="E121">
+        <v>23</v>
+      </c>
+      <c r="F121">
+        <v>4.9356223175965663</v>
+      </c>
+      <c r="H121" s="18" t="s">
+        <v>9</v>
+      </c>
+      <c r="I121">
+        <v>11</v>
+      </c>
+      <c r="J121">
+        <v>6.1452513966480442</v>
+      </c>
+    </row>
+    <row r="122" spans="4:14" x14ac:dyDescent="0.3">
+      <c r="D122" s="18" t="s">
+        <v>13</v>
+      </c>
+      <c r="E122">
+        <v>6</v>
+      </c>
+      <c r="F122">
+        <v>1.2875536480686696</v>
+      </c>
+      <c r="H122" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="I122">
+        <v>2</v>
+      </c>
+      <c r="J122">
+        <v>1.1173184357541899</v>
+      </c>
+    </row>
+    <row r="123" spans="4:14" x14ac:dyDescent="0.3">
+      <c r="D123" s="18" t="s">
+        <v>20</v>
+      </c>
+      <c r="E123">
+        <v>9</v>
+      </c>
+      <c r="F123">
+        <v>1.9313304721030045</v>
+      </c>
+      <c r="H123" s="18" t="s">
+        <v>13</v>
+      </c>
+      <c r="I123">
+        <v>2</v>
+      </c>
+      <c r="J123">
+        <v>1.1173184357541899</v>
+      </c>
+    </row>
+    <row r="124" spans="4:14" x14ac:dyDescent="0.3">
+      <c r="D124" s="18" t="s">
+        <v>12</v>
+      </c>
+      <c r="E124">
+        <v>5</v>
+      </c>
+      <c r="F124">
+        <v>1.0729613733905579</v>
+      </c>
+      <c r="I124">
+        <v>179</v>
+      </c>
+      <c r="J124">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="125" spans="4:14" x14ac:dyDescent="0.3">
+      <c r="D125" s="18" t="s">
+        <v>19</v>
+      </c>
+      <c r="E125">
+        <v>2</v>
+      </c>
+      <c r="F125">
+        <v>0.42918454935622319</v>
+      </c>
+    </row>
+    <row r="126" spans="4:14" x14ac:dyDescent="0.3">
+      <c r="D126" s="18" t="s">
+        <v>23</v>
+      </c>
+      <c r="E126">
+        <v>1</v>
+      </c>
+      <c r="F126">
+        <v>0.21459227467811159</v>
+      </c>
+    </row>
+    <row r="127" spans="4:14" x14ac:dyDescent="0.3">
+      <c r="E127">
+        <v>466</v>
+      </c>
+      <c r="F127">
         <v>100</v>
       </c>
     </row>

</xml_diff>